<commit_message>
updated "Graduate Students" sheet
</commit_message>
<xml_diff>
--- a/data/George-Mason-U.xlsx
+++ b/data/George-Mason-U.xlsx
@@ -7454,7 +7454,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>All part-time studentsAll full-time students</t>
+          <t>All students</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -7491,7 +7491,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">    MaleMale</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -7528,7 +7528,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    FemaleFemale</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -7565,7 +7565,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  U.S. citizens and permanent residentsU.S. citizens and permanent residents</t>
+          <t>U.S. citizens and permanent residents</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -7602,7 +7602,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Hispanic or LatinoHispanic or Latino</t>
+          <t>Hispanic or Latino</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -7639,7 +7639,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Not Hispanic or LatinoNot Hispanic or Latino</t>
+          <t>Not Hispanic or Latino</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -7676,7 +7676,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">      American Indian or Alaska NativeAmerican Indian or Alaska Native</t>
+          <t>American Indian or Alaska Native</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -7713,7 +7713,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">      AsianAsian</t>
+          <t>Asian</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -7750,7 +7750,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Black or African AmericanBlack or African American</t>
+          <t>Black or African American</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -7787,7 +7787,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Native Hawaiian or Other Pacific IslanderNative Hawaiian or Other Pacific Islander</t>
+          <t>Native Hawaiian or Other Pacific Islander</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -7824,7 +7824,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">      WhiteWhite</t>
+          <t>White</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -7861,7 +7861,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">      More than one raceMore than one race</t>
+          <t>More than one race</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -7898,7 +7898,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Unknown ethnicity and raceUnknown ethnicity and race</t>
+          <t>Unknown ethnicity and race</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -7935,7 +7935,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Temporary visa holdersTemporary visa holders</t>
+          <t>Temporary visa holders</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -7972,7 +7972,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Science and engineeringScience and engineering</t>
+          <t>Science and engineering</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -8009,7 +8009,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">    ScienceScience</t>
+          <t>Science</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -8046,7 +8046,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Agricultural and veterinary sciencesAgricultural and veterinary sciences</t>
+          <t>Agricultural and veterinary sciences</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -8083,7 +8083,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Biological and biomedical sciencesBiological and biomedical sciences</t>
+          <t>Biological and biomedical sciences</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -8120,7 +8120,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve">      CommunicationCommunication</t>
+          <t>Communication</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -8157,7 +8157,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Computer and information sciencesComputer and information sciences</t>
+          <t>Computer and information sciences</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -8194,7 +8194,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Family and consumer sciences and human sciencesFamily and consumer sciences and human sciences</t>
+          <t>Family and consumer sciences and human sciences</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -8231,7 +8231,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Geosciences, atmospheric sciences, and ocean sciencesGeosciences, atmospheric sciences, and ocean sciences</t>
+          <t>Geosciences, atmospheric sciences, and ocean sciences</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -8268,7 +8268,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Mathematics and statisticsMathematics and statistics</t>
+          <t>Mathematics and statistics</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -8305,7 +8305,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Multidisciplinary and interdisciplinary studiesMultidisciplinary and interdisciplinary studies</t>
+          <t>Multidisciplinary and interdisciplinary studies</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -8342,7 +8342,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Natural resources and conservationNatural resources and conservation</t>
+          <t>Natural resources and conservation</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -8379,7 +8379,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Neurobiology and neuroscienceNeurobiology and neuroscience</t>
+          <t>Neurobiology and neuroscience</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -8416,7 +8416,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Physical sciencesPhysical sciences</t>
+          <t>Physical sciences</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -8453,7 +8453,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t xml:space="preserve">      PsychologyPsychology</t>
+          <t>Psychology</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -8490,7 +8490,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Social sciencesSocial sciences</t>
+          <t>Social sciences</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -8527,7 +8527,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve">    EngineeringEngineering</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -8564,7 +8564,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Aerospace, aeronautical, and astronautical engineeringAerospace, aeronautical, and astronautical engineering</t>
+          <t>Aerospace, aeronautical, and astronautical engineering</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -8601,7 +8601,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Biological, biomedical, and biosystems engineeringBiological, biomedical, and biosystems engineering</t>
+          <t>Biological, biomedical, and biosystems engineering</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -8638,7 +8638,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Chemical, petroleum, and chemical-related engineeringChemical, petroleum, and chemical-related engineering</t>
+          <t>Chemical, petroleum, and chemical-related engineering</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -8675,7 +8675,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Civil, environmental, transportation and related engineering fieldsCivil, environmental, transportation and related engineering fields</t>
+          <t>Civil, environmental, transportation and related engineering fields</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -8712,7 +8712,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Electrical, electronics, communications and computer engineeringElectrical, electronics, communications and computer engineering</t>
+          <t>Electrical, electronics, communications and computer engineering</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -8749,7 +8749,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Industrial, manufacturing, systems engineering and operations researchIndustrial, manufacturing, systems engineering and operations research</t>
+          <t>Industrial, manufacturing, systems engineering and operations research</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -8786,7 +8786,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Mechanical engineeringMechanical engineering</t>
+          <t>Mechanical engineering</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -8823,7 +8823,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Metallurgical, mining, materials and related engineering fieldsMetallurgical, mining, materials and related engineering fields</t>
+          <t>Metallurgical, mining, materials and related engineering fields</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -8860,7 +8860,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Other engineeringOther engineering</t>
+          <t>Other engineering</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -8897,7 +8897,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t xml:space="preserve">    HealthHealth</t>
+          <t>Health</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -8934,7 +8934,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Clinical medicineClinical medicine</t>
+          <t>Clinical medicine</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -8971,7 +8971,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t xml:space="preserve">      Other healthOther health</t>
+          <t>Other health</t>
         </is>
       </c>
       <c r="B43" t="n">

</xml_diff>